<commit_message>
Reverse bias protection dioded added. Mounting holes coutout added
</commit_message>
<xml_diff>
--- a/DecoLED_PCB/Project Outputs for DecoLED_PCB/DecoLED_PCB_BOM_rev_1.2.xlsx
+++ b/DecoLED_PCB/Project Outputs for DecoLED_PCB/DecoLED_PCB_BOM_rev_1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javi_\GitHub\LED_Driver_Deco\DecoLED_PCB\Project Outputs for DecoLED_PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{161E7A8A-A0D8-43C0-A745-96DBBE5397E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB84E819-040F-402D-B2C2-8F5DF0DCB02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9255" yWindow="930" windowWidth="23550" windowHeight="16410" xr2:uid="{20E3855F-88E6-415C-A962-E8DBAD6240B7}"/>
+    <workbookView xWindow="9255" yWindow="930" windowWidth="23550" windowHeight="16410" xr2:uid="{6521D4FF-A6A4-4E7A-BA7E-0184C68A2F69}"/>
   </bookViews>
   <sheets>
     <sheet name="DecoLED_PCB_BOM_rev_1.2" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
   <si>
     <t>Description</t>
   </si>
@@ -113,6 +113,18 @@
   </si>
   <si>
     <t>CN2</t>
+  </si>
+  <si>
+    <t>Schottky Diode</t>
+  </si>
+  <si>
+    <t>RB715UMTL</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>DAN217UMTL</t>
   </si>
   <si>
     <t>Integrated Circuit</t>
@@ -569,8 +581,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877F3703-0689-4F85-9D8F-15EB2D145F1B}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFB061C-61B4-40E7-9A8B-9F195EDB8068}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -728,19 +740,17 @@
       <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>34</v>
@@ -748,35 +758,37 @@
       <c r="C9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="E9" s="1">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>41</v>
@@ -804,7 +816,7 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>47</v>
@@ -820,14 +832,32 @@
       <c r="C13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>49</v>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Diode added to the BOM
</commit_message>
<xml_diff>
--- a/DecoLED_PCB/Project Outputs for DecoLED_PCB/DecoLED_PCB_BOM_rev_1.2.xlsx
+++ b/DecoLED_PCB/Project Outputs for DecoLED_PCB/DecoLED_PCB_BOM_rev_1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javi_\GitHub\LED_Driver_Deco\DecoLED_PCB\Project Outputs for DecoLED_PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB84E819-040F-402D-B2C2-8F5DF0DCB02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F7A9342-9A29-4151-928E-40EABF20AA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9255" yWindow="930" windowWidth="23550" windowHeight="16410" xr2:uid="{6521D4FF-A6A4-4E7A-BA7E-0184C68A2F69}"/>
+    <workbookView xWindow="9255" yWindow="930" windowWidth="23550" windowHeight="16410" xr2:uid="{788CCB81-B0E2-4F6E-9C5D-74D85529359B}"/>
   </bookViews>
   <sheets>
     <sheet name="DecoLED_PCB_BOM_rev_1.2" sheetId="1" r:id="rId1"/>
@@ -581,7 +581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFB061C-61B4-40E7-9A8B-9F195EDB8068}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FBC7DD-32CC-41FF-B1F5-AD88EBB41FC5}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>